<commit_message>
Add to Gantt chart
</commit_message>
<xml_diff>
--- a/gantt-original.xlsx
+++ b/gantt-original.xlsx
@@ -5,26 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7e1bad9ed54c1c6/local/source/2sd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timmy\OneDrive\local\source\2sd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Week</t>
   </si>
@@ -42,6 +37,132 @@
   </si>
   <si>
     <t>Term 4</t>
+  </si>
+  <si>
+    <t>Game Framework</t>
+  </si>
+  <si>
+    <t>Research &amp; test existing libraries</t>
+  </si>
+  <si>
+    <t>Library helpers</t>
+  </si>
+  <si>
+    <t>Game Design</t>
+  </si>
+  <si>
+    <t>General style/genre/type</t>
+  </si>
+  <si>
+    <t>Mechanics</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Project description</t>
+  </si>
+  <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>Pseudocode</t>
+  </si>
+  <si>
+    <t>Initial Gantt chart</t>
+  </si>
+  <si>
+    <t>Final Gantt chart</t>
+  </si>
+  <si>
+    <t>User manual</t>
+  </si>
+  <si>
+    <t>Topic permission</t>
+  </si>
+  <si>
+    <t>Exising game research</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Base runtime (game loop)</t>
+  </si>
+  <si>
+    <t>User input</t>
+  </si>
+  <si>
+    <t>Multimedia</t>
+  </si>
+  <si>
+    <t>Sound Effects</t>
+  </si>
+  <si>
+    <t>Background Music</t>
+  </si>
+  <si>
+    <t>Character Design</t>
+  </si>
+  <si>
+    <t>World Design</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>!</t>
   </si>
 </sst>
 </file>
@@ -97,24 +218,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -390,62 +523,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:AH31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="2" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="3" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -575,17 +709,281 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" t="s">
+        <v>41</v>
+      </c>
+      <c r="N26" t="s">
+        <v>40</v>
+      </c>
+      <c r="O26" t="s">
+        <v>36</v>
+      </c>
+      <c r="P26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>34</v>
+      </c>
+      <c r="R26" t="s">
+        <v>33</v>
+      </c>
+      <c r="S26" t="s">
+        <v>33</v>
+      </c>
+      <c r="T26" t="s">
+        <v>32</v>
+      </c>
+      <c r="U26" t="s">
+        <v>34</v>
+      </c>
+      <c r="V26" t="s">
+        <v>40</v>
+      </c>
+      <c r="W26" t="s">
+        <v>44</v>
+      </c>
+      <c r="X26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="L1:U1"/>
-    <mergeCell ref="X1:AF1"/>
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
+  <conditionalFormatting sqref="B3:AF3 AG26 AI26 B8:AF31 D4:AF7">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(B3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Work on Gantt chart
</commit_message>
<xml_diff>
--- a/gantt-original.xlsx
+++ b/gantt-original.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>Week</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Game Design</t>
   </si>
   <si>
-    <t>General style/genre/type</t>
-  </si>
-  <si>
     <t>Mechanics</t>
   </si>
   <si>
@@ -163,6 +160,24 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>Resource manager</t>
+  </si>
+  <si>
+    <t>Entity system</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Game Content</t>
+  </si>
+  <si>
+    <t>General game genre</t>
+  </si>
+  <si>
+    <t>Graphics Style</t>
   </si>
 </sst>
 </file>
@@ -523,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH31"/>
+  <dimension ref="A1:AH36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,267 +734,340 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>26</v>
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
+      <c r="A21" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>14</v>
+      <c r="A24" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J26" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" t="s">
-        <v>41</v>
-      </c>
-      <c r="M26" t="s">
-        <v>41</v>
-      </c>
-      <c r="N26" t="s">
-        <v>40</v>
-      </c>
-      <c r="O26" t="s">
-        <v>36</v>
-      </c>
-      <c r="P26" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>34</v>
-      </c>
-      <c r="R26" t="s">
-        <v>33</v>
-      </c>
-      <c r="S26" t="s">
-        <v>33</v>
-      </c>
-      <c r="T26" t="s">
-        <v>32</v>
-      </c>
-      <c r="U26" t="s">
-        <v>34</v>
-      </c>
-      <c r="V26" t="s">
-        <v>40</v>
-      </c>
-      <c r="W26" t="s">
-        <v>44</v>
-      </c>
-      <c r="X26" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE26" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>18</v>
+      <c r="A28" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="I29" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" t="s">
+        <v>38</v>
+      </c>
+      <c r="K30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L30" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" t="s">
+        <v>39</v>
+      </c>
+      <c r="O30" t="s">
+        <v>35</v>
+      </c>
+      <c r="P30" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>33</v>
+      </c>
+      <c r="R30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S30" t="s">
+        <v>32</v>
+      </c>
+      <c r="T30" t="s">
+        <v>31</v>
+      </c>
+      <c r="U30" t="s">
+        <v>33</v>
+      </c>
+      <c r="V30" t="s">
+        <v>39</v>
+      </c>
+      <c r="W30" t="s">
+        <v>43</v>
+      </c>
+      <c r="X30" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="J32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AF3 AG26 AI26 B8:AF31 D4:AF7">
+  <conditionalFormatting sqref="B3:AF3 AG30 AI30 B9:AF36 D4:AF8">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Finish original gantt chart
</commit_message>
<xml_diff>
--- a/gantt-original.xlsx
+++ b/gantt-original.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+  <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timmy\OneDrive\local\source\2sd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="63">
   <si>
     <t>Week</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Mechanics</t>
   </si>
   <si>
-    <t>Levels</t>
-  </si>
-  <si>
     <t>Tutorial</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>Entity system</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Game Content</t>
   </si>
   <si>
@@ -178,12 +172,48 @@
   </si>
   <si>
     <t>Graphics Style</t>
+  </si>
+  <si>
+    <t>Sound system</t>
+  </si>
+  <si>
+    <t>Character addition</t>
+  </si>
+  <si>
+    <t>Details/Balances</t>
+  </si>
+  <si>
+    <t>World system</t>
+  </si>
+  <si>
+    <t>Fixing and Debugging</t>
+  </si>
+  <si>
+    <t>Alpha testing</t>
+  </si>
+  <si>
+    <t>Beta (public) testing</t>
+  </si>
+  <si>
+    <t>Documentation finalisation</t>
+  </si>
+  <si>
+    <t>Testing Data</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>Game pprogression</t>
+  </si>
+  <si>
+    <t>Saves</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -538,19 +568,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH36"/>
+  <dimension ref="A1:AH46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomLeft" activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
@@ -593,7 +623,7 @@
       <c r="AE1" s="5"/>
       <c r="AF1" s="5"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -724,350 +754,568 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="U12" t="s">
+        <v>21</v>
+      </c>
+      <c r="V12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="X13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="X15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R18" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="X19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" t="s">
+        <v>21</v>
+      </c>
+      <c r="S27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="L9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="V31" t="s">
+        <v>21</v>
+      </c>
+      <c r="W31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="V32" t="s">
+        <v>21</v>
+      </c>
+      <c r="W32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="R34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="P35" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" t="s">
+        <v>31</v>
+      </c>
+      <c r="J39" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M39" t="s">
+        <v>39</v>
+      </c>
+      <c r="N39" t="s">
+        <v>38</v>
+      </c>
+      <c r="O39" t="s">
+        <v>34</v>
+      </c>
+      <c r="P39" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>32</v>
+      </c>
+      <c r="R39" t="s">
+        <v>31</v>
+      </c>
+      <c r="S39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="U39" t="s">
+        <v>32</v>
+      </c>
+      <c r="V39" t="s">
+        <v>38</v>
+      </c>
+      <c r="W39" t="s">
+        <v>42</v>
+      </c>
+      <c r="X39" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" t="s">
-        <v>32</v>
-      </c>
-      <c r="I30" t="s">
-        <v>32</v>
-      </c>
-      <c r="J30" t="s">
-        <v>38</v>
-      </c>
-      <c r="K30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L30" t="s">
-        <v>40</v>
-      </c>
-      <c r="M30" t="s">
-        <v>40</v>
-      </c>
-      <c r="N30" t="s">
-        <v>39</v>
-      </c>
-      <c r="O30" t="s">
-        <v>35</v>
-      </c>
-      <c r="P30" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>33</v>
-      </c>
-      <c r="R30" t="s">
-        <v>32</v>
-      </c>
-      <c r="S30" t="s">
-        <v>32</v>
-      </c>
-      <c r="T30" t="s">
-        <v>31</v>
-      </c>
-      <c r="U30" t="s">
-        <v>33</v>
-      </c>
-      <c r="V30" t="s">
-        <v>39</v>
-      </c>
-      <c r="W30" t="s">
-        <v>43</v>
-      </c>
-      <c r="X30" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="V40" t="s">
+        <v>21</v>
+      </c>
+      <c r="W40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="V41" t="s">
+        <v>21</v>
+      </c>
+      <c r="W41" t="s">
+        <v>21</v>
+      </c>
+      <c r="X41" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>49</v>
-      </c>
-      <c r="J32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="E42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>17</v>
       </c>
-      <c r="E33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="AD43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>18</v>
       </c>
-      <c r="AD34" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="AA44" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" t="s">
-        <v>22</v>
+      <c r="M46" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AF3 AG30 AI30 B9:AF36 D4:AF8">
+  <conditionalFormatting sqref="B3:AF3 AG39 AI39 B10:C11 F4:AF11 B33:AF46 B31:J32 M31:AF32 B12:AF30">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>

</xml_diff>